<commit_message>
Make BGF-N PB as in simapro
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_BiogeochemicalFlows_N.xlsx
+++ b/src/aesa_pbs/data/aesa_BiogeochemicalFlows_N.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\bw_methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05FE0A9-99DC-4256-ACBA-14057D2952E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CC1AEC-4304-4C07-88B2-F6DFDA3A2E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,12 +66,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,9 +92,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,7 +379,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,8 +418,8 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>2.44E-8</v>
+      <c r="C3" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>